<commit_message>
20210803 CRE21-011	To revise the sampling criteria for post payment check report PPC0003
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/PPC0003-Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/PPC0003-Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2021\CRE21-004 (Randomise sorting of tx in PPC0002 and PPC0003)\Front-end (Phase 3)\ExcelGenerator\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2021\CRE21-011 (PPC0003 sampling criteria)\Front-end\ExcelGenerator\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>Sub Report ID</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -190,6 +190,18 @@
   </si>
   <si>
     <t>2021/06/24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CRE21-011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To revise the sampling criteria for post payment check report PPC0003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021/08/03</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1158,7 +1170,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1247,6 +1259,20 @@
         <v>46</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="38">
+        <v>5</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>